<commit_message>
Added mean absolute error and max error to every  notebook in /concrete folder
</commit_message>
<xml_diff>
--- a/energy/ENB2012_data.xlsx
+++ b/energy/ENB2012_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Relative Compactness</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wall Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roof Area</t>
   </si>
   <si>
     <t xml:space="preserve">Overall Height</t>
@@ -549,7 +552,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,22 +575,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>

</xml_diff>